<commit_message>
Updated BOM ... added total cost.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t xml:space="preserve">unit cost</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.mcmaster.com/91251A539/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
@@ -155,6 +158,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -176,6 +180,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -327,20 +332,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="70.76"/>
   </cols>
@@ -641,6 +646,15 @@
       </c>
       <c r="I12" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <f aca="false">SUM(F3:F12)</f>
+        <v>46.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>